<commit_message>
updates to excel file and notebook
</commit_message>
<xml_diff>
--- a/data/part_1_df_title_subset.xlsx
+++ b/data/part_1_df_title_subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDC8F94-8439-B44A-B611-7C9FD2FF772C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB955A5-5152-E547-A6B3-D7577111F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="760" windowWidth="20260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="860" windowWidth="26880" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="title_subset_analysis" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3354" uniqueCount="673">
   <si>
     <t>type</t>
   </si>
@@ -2464,16 +2464,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="114.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="16.83203125" customWidth="1"/>
@@ -2551,6 +2551,9 @@
       <c r="H2" t="s">
         <v>598</v>
       </c>
+      <c r="I2" t="s">
+        <v>595</v>
+      </c>
       <c r="J2" t="s">
         <v>591</v>
       </c>
@@ -2563,6 +2566,9 @@
       <c r="M2" t="s">
         <v>612</v>
       </c>
+      <c r="N2" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="3" spans="1:15" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -2603,6 +2609,9 @@
       </c>
       <c r="M3" t="s">
         <v>612</v>
+      </c>
+      <c r="N3" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="64" x14ac:dyDescent="0.2">
@@ -2630,6 +2639,9 @@
       <c r="H4" t="s">
         <v>598</v>
       </c>
+      <c r="I4" t="s">
+        <v>598</v>
+      </c>
       <c r="J4" t="s">
         <v>591</v>
       </c>
@@ -2641,6 +2653,9 @@
       </c>
       <c r="M4" t="s">
         <v>592</v>
+      </c>
+      <c r="N4" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2668,6 +2683,9 @@
       <c r="H5" t="s">
         <v>598</v>
       </c>
+      <c r="I5" t="s">
+        <v>598</v>
+      </c>
       <c r="J5" t="s">
         <v>591</v>
       </c>
@@ -2679,6 +2697,9 @@
       </c>
       <c r="M5" t="s">
         <v>592</v>
+      </c>
+      <c r="N5" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2706,6 +2727,9 @@
       <c r="H6" t="s">
         <v>598</v>
       </c>
+      <c r="I6" t="s">
+        <v>598</v>
+      </c>
       <c r="J6" t="s">
         <v>591</v>
       </c>
@@ -2717,6 +2741,9 @@
       </c>
       <c r="M6" t="s">
         <v>592</v>
+      </c>
+      <c r="N6" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="64" x14ac:dyDescent="0.2">
@@ -2758,6 +2785,9 @@
       </c>
       <c r="M7" t="s">
         <v>610</v>
+      </c>
+      <c r="N7" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2785,6 +2815,9 @@
       <c r="H8" t="s">
         <v>598</v>
       </c>
+      <c r="I8" t="s">
+        <v>598</v>
+      </c>
       <c r="J8" t="s">
         <v>591</v>
       </c>
@@ -2796,6 +2829,9 @@
       </c>
       <c r="M8" t="s">
         <v>592</v>
+      </c>
+      <c r="N8" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2823,6 +2859,9 @@
       <c r="H9" t="s">
         <v>598</v>
       </c>
+      <c r="I9" t="s">
+        <v>598</v>
+      </c>
       <c r="J9" t="s">
         <v>591</v>
       </c>
@@ -2834,6 +2873,9 @@
       </c>
       <c r="M9" t="s">
         <v>592</v>
+      </c>
+      <c r="N9" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2861,6 +2903,9 @@
       <c r="H10" t="s">
         <v>598</v>
       </c>
+      <c r="I10" t="s">
+        <v>598</v>
+      </c>
       <c r="J10" t="s">
         <v>591</v>
       </c>
@@ -2872,6 +2917,9 @@
       </c>
       <c r="M10" t="s">
         <v>592</v>
+      </c>
+      <c r="N10" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -2899,6 +2947,9 @@
       <c r="H11" t="s">
         <v>598</v>
       </c>
+      <c r="I11" t="s">
+        <v>598</v>
+      </c>
       <c r="J11" t="s">
         <v>591</v>
       </c>
@@ -2910,6 +2961,9 @@
       </c>
       <c r="M11" t="s">
         <v>596</v>
+      </c>
+      <c r="N11" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -2937,6 +2991,9 @@
       <c r="H12" t="s">
         <v>598</v>
       </c>
+      <c r="I12" t="s">
+        <v>598</v>
+      </c>
       <c r="J12" t="s">
         <v>591</v>
       </c>
@@ -2978,6 +3035,9 @@
       <c r="H13" t="s">
         <v>598</v>
       </c>
+      <c r="I13" t="s">
+        <v>595</v>
+      </c>
       <c r="J13" t="s">
         <v>591</v>
       </c>
@@ -3019,6 +3079,9 @@
       <c r="H14" t="s">
         <v>598</v>
       </c>
+      <c r="I14" t="s">
+        <v>598</v>
+      </c>
       <c r="J14" t="s">
         <v>591</v>
       </c>
@@ -3060,6 +3123,9 @@
       <c r="H15" t="s">
         <v>598</v>
       </c>
+      <c r="I15" t="s">
+        <v>595</v>
+      </c>
       <c r="J15" t="s">
         <v>591</v>
       </c>
@@ -3101,6 +3167,9 @@
       <c r="H16" t="s">
         <v>598</v>
       </c>
+      <c r="I16" t="s">
+        <v>595</v>
+      </c>
       <c r="J16" t="s">
         <v>591</v>
       </c>
@@ -3142,6 +3211,9 @@
       <c r="H17" t="s">
         <v>598</v>
       </c>
+      <c r="I17" t="s">
+        <v>598</v>
+      </c>
       <c r="J17" t="s">
         <v>591</v>
       </c>
@@ -15776,5 +15848,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>